<commit_message>
fixed memory insufficient problem
</commit_message>
<xml_diff>
--- a/monthly_pattern/cbsa2fipsxw.xlsx
+++ b/monthly_pattern/cbsa2fipsxw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/yuhuaw_ad_unc_edu/Documents/Research/UrbanSubcenter/UrbanSubcenter/Table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Dewey_data\monthly_pattern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:40009_{52FCE346-899F-4B32-A807-00CEBA2D576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD444C6-1A93-4E52-99A6-D0ADCED54FF5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49286C15-F8F6-40BE-8A50-4702B17EE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="760" yWindow="760" windowWidth="28800" windowHeight="18850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2590" yWindow="1290" windowWidth="21780" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cbsa2fipsxw" sheetId="1" r:id="rId1"/>
@@ -8345,8 +8345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1883"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A969" workbookViewId="0">
-      <selection activeCell="G993" sqref="G993"/>
+    <sheetView tabSelected="1" topLeftCell="A404" workbookViewId="0">
+      <selection activeCell="E417" sqref="E417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>